<commit_message>
Shedulling apponitment test case
</commit_message>
<xml_diff>
--- a/src/main/java/com/rc/qa/testdata/TestData.xlsx
+++ b/src/main/java/com/rc/qa/testdata/TestData.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="7935" activeTab="1"/>
+    <workbookView windowWidth="20385" windowHeight="7935" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="CleanerData" sheetId="1" r:id="rId1"/>
     <sheet name="ServiceData" sheetId="2" r:id="rId2"/>
+    <sheet name="ApponitmentData" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525" iterate="1" iterateCount="100" iterateDelta="0.001"/>
   <oleSize ref="A1:B2"/>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16">
   <si>
     <t>cleaner_email</t>
   </si>
@@ -46,6 +47,24 @@
   </si>
   <si>
     <t>Update Automated Service</t>
+  </si>
+  <si>
+    <t>Property</t>
+  </si>
+  <si>
+    <t>HK</t>
+  </si>
+  <si>
+    <t>Service</t>
+  </si>
+  <si>
+    <t>Bits New 11</t>
+  </si>
+  <si>
+    <t>Ganesh Mule</t>
+  </si>
+  <si>
+    <t>roof cleaning</t>
   </si>
 </sst>
 </file>
@@ -54,9 +73,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -76,6 +95,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -84,14 +111,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -105,6 +124,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
@@ -128,24 +163,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -167,6 +193,27 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -175,34 +222,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -220,54 +239,168 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -280,127 +413,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -411,6 +430,26 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -425,26 +464,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -474,21 +493,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -511,10 +515,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -532,130 +551,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1022,8 +1041,8 @@
   <sheetPr/>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="2"/>
@@ -1059,4 +1078,47 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="12.1428571428571" customWidth="1"/>
+    <col min="2" max="3" width="13.5714285714286" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Mange regions code edit code
</commit_message>
<xml_diff>
--- a/src/main/java/com/rc/qa/testdata/TestData.xlsx
+++ b/src/main/java/com/rc/qa/testdata/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="7935" activeTab="3"/>
+    <workbookView windowWidth="19890" windowHeight="7935" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="CleanerData" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20">
   <si>
     <t>cleaner_email</t>
   </si>
@@ -71,7 +71,13 @@
     <t>RegionName</t>
   </si>
   <si>
-    <t>Automated Region</t>
+    <t>updateRegionName</t>
+  </si>
+  <si>
+    <t>Automated Region 1</t>
+  </si>
+  <si>
+    <t>Updted Automation Region</t>
   </si>
 </sst>
 </file>
@@ -79,10 +85,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -96,13 +102,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -138,9 +137,47 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -154,9 +191,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -171,6 +208,27 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -179,59 +237,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -246,13 +252,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -264,169 +426,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -437,21 +443,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -481,24 +472,20 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -518,6 +505,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -527,28 +529,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -558,130 +564,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1133,25 +1139,32 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="13.4285714285714" customWidth="1"/>
+    <col min="1" max="1" width="19.1428571428571" customWidth="1"/>
+    <col min="2" max="2" width="27.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>